<commit_message>
added work to link local bank sites with mortgage data
</commit_message>
<xml_diff>
--- a/data/Urban-HMDA_neighborhood_data_codebook.xlsx
+++ b/data/Urban-HMDA_neighborhood_data_codebook.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rob\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kathrynhurchla/Documents/GitHub/real-estate-stats/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDEAD6E1-7D89-4688-BA02-ECA40F5AFA47}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FACE4F2-FBA7-6E49-826E-ED929A45FD31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3480" yWindow="2100" windowWidth="22860" windowHeight="13035" firstSheet="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="49940" yWindow="660" windowWidth="22860" windowHeight="20380" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Readme" sheetId="2" r:id="rId1"/>
@@ -818,34 +818,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:A7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="84.5703125" style="3" customWidth="1"/>
+    <col min="1" max="1" width="84.5" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" ht="32" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" ht="32" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="7" spans="1:1" ht="105" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" ht="96" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>3</v>
       </c>
@@ -860,20 +860,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D61"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
+      <selection pane="bottomLeft" activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.7109375" customWidth="1"/>
-    <col min="4" max="4" width="58.85546875" style="3" customWidth="1"/>
+    <col min="1" max="1" width="4.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.6640625" customWidth="1"/>
+    <col min="3" max="3" width="9.6640625" customWidth="1"/>
+    <col min="4" max="4" width="58.83203125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -887,7 +887,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -901,7 +901,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -915,7 +915,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -929,7 +929,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -943,7 +943,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -957,7 +957,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -971,7 +971,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -985,7 +985,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -999,7 +999,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1013,7 +1013,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1027,7 +1027,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1041,7 +1041,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1055,7 +1055,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1069,7 +1069,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1083,7 +1083,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1097,7 +1097,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1111,7 +1111,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1125,7 +1125,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1139,7 +1139,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1153,7 +1153,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1167,7 +1167,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1181,7 +1181,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1195,7 +1195,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1209,7 +1209,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1223,7 +1223,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1237,7 +1237,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1251,7 +1251,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1265,7 +1265,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1279,7 +1279,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1293,7 +1293,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1307,7 +1307,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1321,7 +1321,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1335,7 +1335,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1349,7 +1349,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1363,7 +1363,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1377,7 +1377,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>36</v>
       </c>
@@ -1391,7 +1391,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>37</v>
       </c>
@@ -1405,7 +1405,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>38</v>
       </c>
@@ -1419,7 +1419,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>39</v>
       </c>
@@ -1433,7 +1433,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>40</v>
       </c>
@@ -1447,7 +1447,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>41</v>
       </c>
@@ -1461,7 +1461,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>42</v>
       </c>
@@ -1475,7 +1475,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>43</v>
       </c>
@@ -1489,7 +1489,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>44</v>
       </c>
@@ -1503,7 +1503,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>45</v>
       </c>
@@ -1517,7 +1517,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>46</v>
       </c>
@@ -1531,7 +1531,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>47</v>
       </c>
@@ -1545,7 +1545,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>48</v>
       </c>
@@ -1559,7 +1559,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>49</v>
       </c>
@@ -1573,7 +1573,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>50</v>
       </c>
@@ -1587,7 +1587,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>51</v>
       </c>
@@ -1601,7 +1601,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>52</v>
       </c>
@@ -1615,7 +1615,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>53</v>
       </c>
@@ -1629,7 +1629,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>54</v>
       </c>
@@ -1643,7 +1643,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>55</v>
       </c>
@@ -1657,7 +1657,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>56</v>
       </c>
@@ -1671,7 +1671,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>57</v>
       </c>
@@ -1685,7 +1685,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="59" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>58</v>
       </c>
@@ -1699,7 +1699,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="60" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>59</v>
       </c>
@@ -1713,7 +1713,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>60</v>
       </c>

</xml_diff>